<commit_message>
User can use Annotation to mark alias.
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,18 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>score</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>张三</t>
   </si>
   <si>
@@ -57,6 +45,18 @@
   </si>
   <si>
     <t>王小五</t>
+  </si>
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>昵称</t>
+  </si>
+  <si>
+    <t>成绩</t>
+  </si>
+  <si>
+    <t>年龄</t>
   </si>
 </sst>
 </file>
@@ -374,31 +374,31 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -409,10 +409,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -423,10 +423,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>100</v>

</xml_diff>